<commit_message>
Update - update Datatest
</commit_message>
<xml_diff>
--- a/DataTesting.xlsx
+++ b/DataTesting.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3 xr6 xr10 x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C085C0-A275-43E5-B338-D57725FCD092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15800" windowWidth="28040" xWindow="4240" yWindow="640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test" sheetId="2" r:id="rId6"/>
+    <sheet name="Test" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcMode="auto"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -32,7 +32,16 @@
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{8CF2D2CA-840E-40B7-8C00-4797A33CB52D}">
       <text>
-        <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: seller_domain/product_link</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: seller_domain/product_link</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -40,29 +49,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t/>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="9.75"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>pbs-ilham+buyer@tokopedia.com</t>
-    </r>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>env</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>product_link</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>courier</t>
+  </si>
+  <si>
+    <t>payment_method</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -80,16 +94,10 @@
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
@@ -109,21 +117,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -133,6 +141,60 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>790575</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="Text Box 2" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1078471-F4B0-4B29-A252-08C2FDA50FD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -444,184 +506,91 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3 xr6 xr10 x15">
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <outlinePr summaryBelow="false" summaryRight="false"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showGridLines="true" tabSelected="true" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14" defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="14" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" max="1" min="1" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="2" min="2" style="0" width="28"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="3" min="3" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="4" min="4" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="5" min="5" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="6" min="6" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="7" min="7" style="0" width="17"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="str">
-        <v>env</v>
-      </c>
-      <c r="B1" s="1" t="str">
-        <v>email</v>
-      </c>
-      <c r="C1" s="1" t="str">
-        <v>password</v>
-      </c>
-      <c r="D1" s="1" t="str">
-        <v>product_link</v>
-      </c>
-      <c r="E1" s="1" t="str">
-        <v>service</v>
-      </c>
-      <c r="F1" s="1" t="str">
-        <v>courier</v>
-      </c>
-      <c r="G1" s="1" t="str">
-        <v>payment_method</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Production</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="str">
-        <v>buyertkpd</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <v>bo-seller/gantungan-kunci-umaru</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Reguler</v>
-      </c>
-      <c r="F2" t="str">
-        <v>SiCepat</v>
-      </c>
-      <c r="G2" t="str">
-        <v>Saldo Tokopedia</v>
-      </c>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Production</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="str">
-        <v>buyertkpd</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <v>bo-seller/gantungan-kunci-umaru</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Same Day 8 Jam</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Whitelabel</v>
-      </c>
-      <c r="G3" t="str">
-        <v>Saldo Tokopedia</v>
-      </c>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Production</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="str">
-        <v>buyertkpd</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <v>bo-seller/gantungan-kunci-umaru</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Ekonomi</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Wahana</v>
-      </c>
-      <c r="G4" t="str">
-        <v>Saldo Tokopedia</v>
-      </c>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Production</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="str">
-        <v>buyertkpd</v>
-      </c>
-      <c r="D5" s="1" t="str">
-        <v>bo-seller/gantungan-kunci-umaru</v>
-      </c>
-      <c r="E5" t="str">
-        <v>Reguler</v>
-      </c>
-      <c r="F5" t="str">
-        <v>JNE</v>
-      </c>
-      <c r="G5" t="str">
-        <v>Saldo Tokopedia</v>
-      </c>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Production</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="str">
-        <v>buyertkpd</v>
-      </c>
-      <c r="D6" s="1" t="str">
-        <v>bo-seller/gantungan-kunci-umaru</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Reguler</v>
-      </c>
-      <c r="F6" t="str">
-        <v>TIKI</v>
-      </c>
-      <c r="G6" t="str">
-        <v>Saldo Tokopedia</v>
-      </c>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" showErrorMessage="true" sqref="A2:A200" type="list">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A200" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Staging,Production"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" showErrorMessage="true" sqref="E2:E200" type="list">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E200" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Instant 3 Jam,Same Day 8 Jam,Same Day,Next Day,Reguler,Kargo,Ekonomi,Kurir Toko"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" showErrorMessage="true" sqref="F2:F200" type="list">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F200" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Whitelabel,Kurir Rekomendasi,SiCepat,AnterAja,Lion Parcel,Ninja Xpress,REX,Paxel,GTL,J&amp;T,JNE,TIKI,Wahana,Pos Indonesia"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B5" display="pbs-ilham+buyer@tokopedia.com" r:id="rId1"/>
-    <hyperlink ref="B2" display="pbs-ilham+buyer@tokopedia.com" r:id="rId2"/>
-    <hyperlink ref="B4" display="pbs-ilham+buyer@tokopedia.com" r:id="rId3"/>
-    <hyperlink ref="B6" display="pbs-ilham+buyer@tokopedia.com" r:id="rId4"/>
-    <hyperlink ref="B3" display="pbs-ilham+buyer@tokopedia.com" r:id="rId5"/>
-  </hyperlinks>
-  <legacyDrawing r:id="rId6"/>
-  <picture r:id="rId9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <picture r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>